<commit_message>
update tien do tuan
</commit_message>
<xml_diff>
--- a/Biên bản làm việc nhóm.xlsx
+++ b/Biên bản làm việc nhóm.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\haui_s6\thuc_tap_chuyen_nganh\Báo cáo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\haui_s6\thuc_tap_chuyen_nganh\HaUI_TTCN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA21008-3E46-4776-8A8A-7B52349B9A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F265F840-26A7-44E3-BD46-E73E482C9DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CE8FA7BD-5558-4429-933A-1A849615429B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CE8FA7BD-5558-4429-933A-1A849615429B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tuần 1" sheetId="1" r:id="rId1"/>
     <sheet name="Tuần 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tuần 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="90">
   <si>
     <t>Biên bản họp , làm việc nhóm</t>
   </si>
@@ -282,12 +283,45 @@
   <si>
     <t>Tìm hiểu đăng ký, đăng nhập</t>
   </si>
+  <si>
+    <t>Thời gian - time: 01/04/2023</t>
+  </si>
+  <si>
+    <t>Phát triển một số phương thức get</t>
+  </si>
+  <si>
+    <t>20'</t>
+  </si>
+  <si>
+    <t>Vẽ giao diện trang chi tiết sản phẩm</t>
+  </si>
+  <si>
+    <t>10'</t>
+  </si>
+  <si>
+    <t>Tìm hiểu trang đăng ký, đăng nhập</t>
+  </si>
+  <si>
+    <t>Viết tiếp báo cáo, kế hoạch tuần</t>
+  </si>
+  <si>
+    <t>15'</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa use case hệ thống</t>
+  </si>
+  <si>
+    <t>Viết báo cáo, kế hoạch tuần</t>
+  </si>
+  <si>
+    <t>Hỗ trợ người khác - Support other(s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +366,25 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -347,7 +400,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -837,11 +890,99 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -958,6 +1099,108 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -965,12 +1208,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1015,27 +1252,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1046,119 +1262,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1181,7 +1298,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1193,13 +1340,190 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1684,14 +2008,14 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1934,14 +2258,14 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="61"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1964,12 +2288,12 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="65"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2004,10 +2328,10 @@
       <c r="D15" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="66" t="s">
+      <c r="E15" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="67"/>
+      <c r="F15" s="92"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -2042,10 +2366,10 @@
       <c r="D16" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="68" t="s">
+      <c r="E16" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="69"/>
+      <c r="F16" s="94"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -2080,10 +2404,10 @@
       <c r="D17" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="E17" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="71"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -2106,22 +2430,22 @@
       <c r="Z17" s="7"/>
     </row>
     <row r="18" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47">
+      <c r="A18" s="79">
         <v>3</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="44"/>
+      <c r="F18" s="69"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -2144,12 +2468,12 @@
       <c r="Z18" s="7"/>
     </row>
     <row r="19" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="46"/>
+      <c r="A19" s="80"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="78"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -2172,22 +2496,22 @@
       <c r="Z19" s="7"/>
     </row>
     <row r="20" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="43">
+      <c r="A20" s="68">
         <v>4</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="44"/>
+      <c r="F20" s="69"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -2210,12 +2534,12 @@
       <c r="Z20" s="7"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" s="55"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="57"/>
+      <c r="A21" s="87"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="89"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -2238,12 +2562,12 @@
       <c r="Z21" s="7"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A22" s="45"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="78"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -2278,8 +2602,8 @@
       <c r="D23" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="70"/>
-      <c r="F23" s="71"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="67"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -2314,8 +2638,8 @@
       <c r="D24" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="69"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -2350,8 +2674,8 @@
       <c r="D25" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="43"/>
-      <c r="F25" s="44"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="69"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -2408,10 +2732,10 @@
       <c r="B27" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="76" t="s">
+      <c r="C27" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="76"/>
+      <c r="D27" s="70"/>
       <c r="E27" s="18" t="s">
         <v>29</v>
       </c>
@@ -2446,10 +2770,10 @@
       <c r="B28" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="77" t="s">
+      <c r="C28" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="77"/>
+      <c r="D28" s="71"/>
       <c r="E28" s="19" t="s">
         <v>63</v>
       </c>
@@ -2482,10 +2806,10 @@
       <c r="B29" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="77"/>
+      <c r="D29" s="71"/>
       <c r="E29" s="19" t="s">
         <v>66</v>
       </c>
@@ -2518,10 +2842,10 @@
       <c r="B30" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="77" t="s">
+      <c r="C30" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="77"/>
+      <c r="D30" s="71"/>
       <c r="E30" s="19" t="s">
         <v>66</v>
       </c>
@@ -2554,10 +2878,10 @@
       <c r="B31" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="42"/>
+      <c r="D31" s="76"/>
       <c r="E31" s="19" t="s">
         <v>66</v>
       </c>
@@ -2584,14 +2908,14 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="78" t="s">
+      <c r="A32" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="79"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="42"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -2614,12 +2938,12 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="62"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="65"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="45"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2654,10 +2978,10 @@
       <c r="D34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="74" t="s">
+      <c r="E34" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="75"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -2680,22 +3004,22 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="80">
+      <c r="A35" s="46">
         <v>1</v>
       </c>
-      <c r="B35" s="82" t="s">
+      <c r="B35" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="84">
+      <c r="C35" s="48">
         <v>45009</v>
       </c>
-      <c r="D35" s="80" t="s">
+      <c r="D35" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="86" t="s">
+      <c r="E35" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="F35" s="87"/>
+      <c r="F35" s="51"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -2718,12 +3042,12 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="90"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="90"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="94"/>
+      <c r="A36" s="57"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="63"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -2746,12 +3070,12 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="81"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="85"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="89"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="53"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -2774,22 +3098,22 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="80">
+      <c r="A38" s="46">
         <v>2</v>
       </c>
-      <c r="B38" s="82" t="s">
+      <c r="B38" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="84">
+      <c r="C38" s="48">
         <v>45009</v>
       </c>
-      <c r="D38" s="80" t="s">
+      <c r="D38" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="86" t="s">
+      <c r="E38" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F38" s="87"/>
+      <c r="F38" s="51"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -2812,12 +3136,12 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="81"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="88"/>
-      <c r="F39" s="89"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="53"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -2840,22 +3164,22 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="80">
+      <c r="A40" s="46">
         <v>3</v>
       </c>
-      <c r="B40" s="80" t="s">
+      <c r="B40" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="84">
+      <c r="C40" s="48">
         <v>45009</v>
       </c>
-      <c r="D40" s="80" t="s">
+      <c r="D40" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="86" t="s">
+      <c r="E40" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="87"/>
+      <c r="F40" s="51"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2878,12 +3202,12 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="81"/>
-      <c r="B41" s="81"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="88"/>
-      <c r="F41" s="89"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="53"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -2906,12 +3230,12 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="59"/>
-      <c r="B42" s="60"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="61"/>
+      <c r="A42" s="54"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="56"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -2934,12 +3258,12 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="62"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
-      <c r="F43" s="65"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="45"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -3130,12 +3454,12 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="78"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="63"/>
-      <c r="D50" s="63"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="79"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="42"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -3158,12 +3482,12 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="62"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="65"/>
+      <c r="A51" s="43"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="45"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -29593,37 +29917,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A50:F51"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="A42:F43"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:F37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:F39"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A32:F33"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="E18:F19"/>
@@ -29640,6 +29933,37 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="A32:F33"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:F39"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:F37"/>
+    <mergeCell ref="A50:F51"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:F41"/>
+    <mergeCell ref="A42:F43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29649,7 +29973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49142C0E-CA9B-4C3E-863C-24BF164051AB}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
@@ -29713,14 +30037,14 @@
       <c r="F5" s="73"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -29823,22 +30147,22 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="61"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="65"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
@@ -29853,144 +30177,144 @@
       <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="75"/>
+      <c r="F15" s="65"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="102">
+      <c r="A16" s="97">
         <v>1</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="97" t="s">
+      <c r="C16" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="80" t="s">
+      <c r="D16" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="86" t="s">
+      <c r="E16" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="87"/>
+      <c r="F16" s="51"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="103"/>
+      <c r="A17" s="114"/>
       <c r="B17" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="94"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="63"/>
     </row>
     <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="104"/>
+      <c r="A18" s="115"/>
       <c r="B18" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="106"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="89"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="53"/>
     </row>
     <row r="19" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="102">
+      <c r="A19" s="97">
         <v>2</v>
       </c>
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="97" t="s">
+      <c r="C19" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="80" t="s">
+      <c r="D19" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="87"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="51"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="121"/>
-      <c r="B20" s="115"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="101"/>
+      <c r="A20" s="98"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="110"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="112"/>
+      <c r="F20" s="113"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="77">
+      <c r="A21" s="71">
         <v>3</v>
       </c>
-      <c r="B21" s="108" t="s">
+      <c r="B21" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="116" t="s">
+      <c r="C21" s="118" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="77" t="s">
+      <c r="D21" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="77"/>
-      <c r="B22" s="109"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="77">
+      <c r="A23" s="71">
         <v>4</v>
       </c>
-      <c r="B23" s="117" t="s">
+      <c r="B23" s="119" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="108" t="s">
+      <c r="C23" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="77" t="s">
+      <c r="D23" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="77"/>
-      <c r="B24" s="118"/>
-      <c r="C24" s="109"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
+      <c r="A24" s="71"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="101"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="77">
+      <c r="A25" s="71">
         <v>5</v>
       </c>
-      <c r="B25" s="119" t="s">
+      <c r="B25" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="108" t="s">
+      <c r="C25" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="108" t="s">
+      <c r="D25" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="111"/>
-      <c r="F25" s="112"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="104"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="77"/>
-      <c r="B26" s="120"/>
-      <c r="C26" s="109"/>
-      <c r="D26" s="110"/>
-      <c r="E26" s="113"/>
-      <c r="F26" s="114"/>
+      <c r="A26" s="71"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="101"/>
+      <c r="D26" s="102"/>
+      <c r="E26" s="105"/>
+      <c r="F26" s="106"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
@@ -30007,10 +30331,10 @@
       <c r="B28" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="76" t="s">
+      <c r="C28" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="76"/>
+      <c r="D28" s="70"/>
       <c r="E28" s="18" t="s">
         <v>29</v>
       </c>
@@ -30023,8 +30347,8 @@
         <v>1</v>
       </c>
       <c r="B29" s="19"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="77"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
     </row>
@@ -30033,8 +30357,8 @@
         <v>2</v>
       </c>
       <c r="B30" s="19"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
     </row>
@@ -30043,8 +30367,8 @@
         <v>3</v>
       </c>
       <c r="B31" s="20"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
     </row>
@@ -30053,28 +30377,28 @@
         <v>4</v>
       </c>
       <c r="B32" s="20"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="76"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="78" t="s">
+      <c r="A33" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="79"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="42"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="78"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="79"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="42"/>
     </row>
     <row r="35" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
@@ -30089,160 +30413,160 @@
       <c r="D35" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="76" t="s">
+      <c r="E35" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="76"/>
+      <c r="F35" s="70"/>
     </row>
     <row r="36" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="77">
+      <c r="A36" s="71">
         <v>1</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="96">
+      <c r="C36" s="121">
         <v>45017</v>
       </c>
-      <c r="D36" s="95" t="s">
+      <c r="D36" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="71"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="77"/>
+      <c r="A37" s="71"/>
       <c r="B37" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="96"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
+      <c r="C37" s="121"/>
+      <c r="D37" s="108"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
     </row>
     <row r="38" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="77"/>
+      <c r="A38" s="71"/>
       <c r="B38" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="96"/>
-      <c r="D38" s="95"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
+      <c r="C38" s="121"/>
+      <c r="D38" s="108"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="77">
+      <c r="A39" s="71">
         <v>2</v>
       </c>
-      <c r="B39" s="115" t="s">
+      <c r="B39" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="96">
+      <c r="C39" s="121">
         <v>45017</v>
       </c>
-      <c r="D39" s="95" t="s">
+      <c r="D39" s="108" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="77"/>
-      <c r="F39" s="77"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
     </row>
     <row r="40" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="77"/>
-      <c r="B40" s="115"/>
-      <c r="C40" s="96"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="77"/>
+      <c r="A40" s="71"/>
+      <c r="B40" s="99"/>
+      <c r="C40" s="121"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="71"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="77">
+      <c r="A41" s="71">
         <v>3</v>
       </c>
-      <c r="B41" s="77" t="s">
+      <c r="B41" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="96">
+      <c r="C41" s="121">
         <v>45017</v>
       </c>
-      <c r="D41" s="95" t="s">
+      <c r="D41" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="77"/>
-      <c r="F41" s="77"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="77"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="96"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="77"/>
+      <c r="A42" s="71"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="121"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="77">
+      <c r="A43" s="71">
         <v>4</v>
       </c>
       <c r="B43" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="96">
+      <c r="C43" s="121">
         <v>45017</v>
       </c>
-      <c r="D43" s="95" t="s">
+      <c r="D43" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="77"/>
-      <c r="F43" s="77"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="77"/>
+      <c r="A44" s="71"/>
       <c r="B44" s="107"/>
-      <c r="C44" s="96"/>
-      <c r="D44" s="77"/>
-      <c r="E44" s="77"/>
-      <c r="F44" s="77"/>
+      <c r="C44" s="121"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="71"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="77">
+      <c r="A45" s="71">
         <v>5</v>
       </c>
-      <c r="B45" s="95" t="s">
+      <c r="B45" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="96">
+      <c r="C45" s="121">
         <v>45017</v>
       </c>
-      <c r="D45" s="95" t="s">
+      <c r="D45" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="77"/>
-      <c r="F45" s="77"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="71"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="77"/>
-      <c r="B46" s="95"/>
-      <c r="C46" s="96"/>
-      <c r="D46" s="77"/>
-      <c r="E46" s="77"/>
-      <c r="F46" s="77"/>
+      <c r="A46" s="71"/>
+      <c r="B46" s="108"/>
+      <c r="C46" s="121"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="71"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="78" t="s">
+      <c r="A47" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="79"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="42"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="62"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="65"/>
+      <c r="A48" s="43"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="45"/>
     </row>
     <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="35" t="s">
@@ -30355,22 +30679,22 @@
       <c r="F54" s="16"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="78" t="s">
+      <c r="A55" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B55" s="63"/>
-      <c r="C55" s="63"/>
-      <c r="D55" s="63"/>
-      <c r="E55" s="63"/>
-      <c r="F55" s="79"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="42"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="62"/>
-      <c r="B56" s="64"/>
-      <c r="C56" s="64"/>
-      <c r="D56" s="64"/>
-      <c r="E56" s="64"/>
-      <c r="F56" s="65"/>
+      <c r="A56" s="43"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="45"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
@@ -30458,18 +30782,39 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="E21:F22"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E36:F38"/>
+    <mergeCell ref="E39:F40"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:F18"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A41:A42"/>
     <mergeCell ref="A47:F48"/>
     <mergeCell ref="A55:F56"/>
     <mergeCell ref="A25:A26"/>
@@ -30486,43 +30831,832 @@
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="E21:F22"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="E23:F24"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:F20"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:F18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA17D19-DC51-42E0-BBCB-DC80E3016D8D}">
+  <dimension ref="A1:F58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="136" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="137" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="137" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="137" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="137"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="137" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="137"/>
+      <c r="C5" s="137"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
+      <c r="F5" s="137"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="138" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="138"/>
+      <c r="C6" s="138"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
+    </row>
+    <row r="7" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="122" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="122" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="122" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="122" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="122" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="122" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="123">
+        <v>1</v>
+      </c>
+      <c r="B8" s="123" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="123">
+        <v>2</v>
+      </c>
+      <c r="B9" s="123" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="123">
+        <v>3</v>
+      </c>
+      <c r="B10" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="123">
+        <v>4</v>
+      </c>
+      <c r="B11" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="123"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="123">
+        <v>5</v>
+      </c>
+      <c r="B12" s="123" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="139" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="140"/>
+      <c r="C13" s="140"/>
+      <c r="D13" s="140"/>
+      <c r="E13" s="140"/>
+      <c r="F13" s="140"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="141"/>
+      <c r="B14" s="142"/>
+      <c r="C14" s="142"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="142"/>
+      <c r="F14" s="142"/>
+    </row>
+    <row r="15" spans="1:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="A15" s="125" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="126" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="127" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="122" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="143" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="144"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="145">
+        <v>1</v>
+      </c>
+      <c r="B16" s="148" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="151" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="154" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="157"/>
+      <c r="F16" s="158"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="146"/>
+      <c r="B17" s="149"/>
+      <c r="C17" s="152"/>
+      <c r="D17" s="155"/>
+      <c r="E17" s="159"/>
+      <c r="F17" s="160"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="146"/>
+      <c r="B18" s="149"/>
+      <c r="C18" s="153"/>
+      <c r="D18" s="155"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="160"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="146"/>
+      <c r="B19" s="149"/>
+      <c r="C19" s="163" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="155"/>
+      <c r="E19" s="159"/>
+      <c r="F19" s="160"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="147"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="156"/>
+      <c r="E20" s="161"/>
+      <c r="F20" s="162"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="165">
+        <v>2</v>
+      </c>
+      <c r="B21" s="166" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="151" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="165" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="157"/>
+      <c r="F21" s="158"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="156"/>
+      <c r="B22" s="167"/>
+      <c r="C22" s="153"/>
+      <c r="D22" s="156"/>
+      <c r="E22" s="161"/>
+      <c r="F22" s="162"/>
+    </row>
+    <row r="23" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="165">
+        <v>3</v>
+      </c>
+      <c r="B23" s="148" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="165" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="165" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="157"/>
+      <c r="F23" s="158"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="156"/>
+      <c r="B24" s="150"/>
+      <c r="C24" s="156"/>
+      <c r="D24" s="156"/>
+      <c r="E24" s="161"/>
+      <c r="F24" s="162"/>
+    </row>
+    <row r="25" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="165">
+        <v>4</v>
+      </c>
+      <c r="B25" s="128" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="165" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="165" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="157"/>
+      <c r="F25" s="168"/>
+    </row>
+    <row r="26" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="156"/>
+      <c r="B26" s="128" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="155"/>
+      <c r="D26" s="155"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="169"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="129"/>
+      <c r="B27" s="124"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="130"/>
+    </row>
+    <row r="28" spans="1:6" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="131" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="131" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="170" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="171"/>
+      <c r="E28" s="131" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="131" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="132">
+        <v>1</v>
+      </c>
+      <c r="B29" s="132"/>
+      <c r="C29" s="172"/>
+      <c r="D29" s="173"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="132"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="132">
+        <v>2</v>
+      </c>
+      <c r="B30" s="132"/>
+      <c r="C30" s="172"/>
+      <c r="D30" s="173"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="132"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="132">
+        <v>3</v>
+      </c>
+      <c r="B31" s="133"/>
+      <c r="C31" s="172"/>
+      <c r="D31" s="173"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="132"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="132">
+        <v>4</v>
+      </c>
+      <c r="B32" s="133"/>
+      <c r="C32" s="172"/>
+      <c r="D32" s="173"/>
+      <c r="E32" s="132"/>
+      <c r="F32" s="132"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="174" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="175"/>
+      <c r="C33" s="175"/>
+      <c r="D33" s="175"/>
+      <c r="E33" s="175"/>
+      <c r="F33" s="175"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="176"/>
+      <c r="B34" s="177"/>
+      <c r="C34" s="177"/>
+      <c r="D34" s="177"/>
+      <c r="E34" s="177"/>
+      <c r="F34" s="177"/>
+    </row>
+    <row r="35" spans="1:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="A35" s="131" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="131" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="131" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="131" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="170" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="171"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="148">
+        <v>1</v>
+      </c>
+      <c r="B36" s="148" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="178">
+        <v>45142</v>
+      </c>
+      <c r="D36" s="151" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="157"/>
+      <c r="F36" s="158"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="149"/>
+      <c r="B37" s="149"/>
+      <c r="C37" s="179"/>
+      <c r="D37" s="152"/>
+      <c r="E37" s="159"/>
+      <c r="F37" s="160"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="149"/>
+      <c r="B38" s="149"/>
+      <c r="C38" s="179"/>
+      <c r="D38" s="153"/>
+      <c r="E38" s="159"/>
+      <c r="F38" s="160"/>
+    </row>
+    <row r="39" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="149"/>
+      <c r="B39" s="149"/>
+      <c r="C39" s="179"/>
+      <c r="D39" s="151" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="159"/>
+      <c r="F39" s="160"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="150"/>
+      <c r="B40" s="150"/>
+      <c r="C40" s="180"/>
+      <c r="D40" s="153"/>
+      <c r="E40" s="161"/>
+      <c r="F40" s="162"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="165">
+        <v>2</v>
+      </c>
+      <c r="B41" s="166" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="178">
+        <v>45142</v>
+      </c>
+      <c r="D41" s="151" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="157"/>
+      <c r="F41" s="158"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="156"/>
+      <c r="B42" s="167"/>
+      <c r="C42" s="180"/>
+      <c r="D42" s="153"/>
+      <c r="E42" s="161"/>
+      <c r="F42" s="162"/>
+    </row>
+    <row r="43" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="165">
+        <v>3</v>
+      </c>
+      <c r="B43" s="148" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="178">
+        <v>45142</v>
+      </c>
+      <c r="D43" s="151" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" s="157"/>
+      <c r="F43" s="158"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="156"/>
+      <c r="B44" s="150"/>
+      <c r="C44" s="180"/>
+      <c r="D44" s="153"/>
+      <c r="E44" s="161"/>
+      <c r="F44" s="162"/>
+    </row>
+    <row r="45" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="165">
+        <v>4</v>
+      </c>
+      <c r="B45" s="128" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="178">
+        <v>45142</v>
+      </c>
+      <c r="D45" s="151" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45" s="157"/>
+      <c r="F45" s="158"/>
+    </row>
+    <row r="46" spans="1:6" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="156"/>
+      <c r="B46" s="128" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="180"/>
+      <c r="D46" s="153"/>
+      <c r="E46" s="161"/>
+      <c r="F46" s="162"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="174" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" s="175"/>
+      <c r="C47" s="175"/>
+      <c r="D47" s="175"/>
+      <c r="E47" s="175"/>
+      <c r="F47" s="175"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="181"/>
+      <c r="B48" s="182"/>
+      <c r="C48" s="182"/>
+      <c r="D48" s="182"/>
+      <c r="E48" s="182"/>
+      <c r="F48" s="182"/>
+    </row>
+    <row r="49" spans="1:6" ht="93" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="134" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="134" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="134" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="122" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="122" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" s="134" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="135">
+        <v>1</v>
+      </c>
+      <c r="B50" s="123" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="36">
+        <v>1</v>
+      </c>
+      <c r="D50" s="37">
+        <v>2</v>
+      </c>
+      <c r="E50" s="37">
+        <v>2</v>
+      </c>
+      <c r="F50" s="135"/>
+    </row>
+    <row r="51" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="135">
+        <v>2</v>
+      </c>
+      <c r="B51" s="123" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="38">
+        <v>1</v>
+      </c>
+      <c r="D51" s="39">
+        <v>1</v>
+      </c>
+      <c r="E51" s="39">
+        <v>1</v>
+      </c>
+      <c r="F51" s="135"/>
+    </row>
+    <row r="52" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="135">
+        <v>3</v>
+      </c>
+      <c r="B52" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="38">
+        <v>2</v>
+      </c>
+      <c r="D52" s="39">
+        <v>1</v>
+      </c>
+      <c r="E52" s="39">
+        <v>2</v>
+      </c>
+      <c r="F52" s="135"/>
+    </row>
+    <row r="53" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="135">
+        <v>4</v>
+      </c>
+      <c r="B53" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="38">
+        <v>1</v>
+      </c>
+      <c r="D53" s="39">
+        <v>1</v>
+      </c>
+      <c r="E53" s="39">
+        <v>1</v>
+      </c>
+      <c r="F53" s="135"/>
+    </row>
+    <row r="54" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="135">
+        <v>5</v>
+      </c>
+      <c r="B54" s="123" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="38">
+        <v>3</v>
+      </c>
+      <c r="D54" s="39">
+        <v>1</v>
+      </c>
+      <c r="E54" s="39">
+        <v>1</v>
+      </c>
+      <c r="F54" s="135"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="141" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="142"/>
+      <c r="C55" s="142"/>
+      <c r="D55" s="142"/>
+      <c r="E55" s="142"/>
+      <c r="F55" s="142"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="181"/>
+      <c r="B56" s="182"/>
+      <c r="C56" s="182"/>
+      <c r="D56" s="182"/>
+      <c r="E56" s="182"/>
+      <c r="F56" s="182"/>
+    </row>
+    <row r="57" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="122" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="122" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="122" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="122" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57" s="122" t="s">
+        <v>48</v>
+      </c>
+      <c r="F57" s="122"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="123">
+        <v>1</v>
+      </c>
+      <c r="B58" s="123">
+        <v>5</v>
+      </c>
+      <c r="C58" s="123">
+        <v>0</v>
+      </c>
+      <c r="D58" s="123">
+        <v>0</v>
+      </c>
+      <c r="E58" s="123">
+        <v>0</v>
+      </c>
+      <c r="F58" s="123"/>
+    </row>
+  </sheetData>
+  <mergeCells count="57">
+    <mergeCell ref="A47:F48"/>
+    <mergeCell ref="A55:F56"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A33:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:F40"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:F26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:F22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E36:F38"/>
-    <mergeCell ref="E39:F40"/>
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="E23:F24"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D20"/>
+    <mergeCell ref="E16:F20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>